<commit_message>
adjust the node number
</commit_message>
<xml_diff>
--- a/cloudMap_v10.xlsx
+++ b/cloudMap_v10.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/Documents/MAPF/MultiAgentPathFinder/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F26C41-CAD7-4745-9FBD-B3958456F547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="60160" yWindow="16340" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,20 +27,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="2">
   <si>
-    <t xml:space="preserve">axis</t>
+    <t>axis</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -44,19 +46,10 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="5">
@@ -86,110 +79,93 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="hair"/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -248,124 +224,432 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333F50"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="10.67"/>
+    <col min="4" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="n">
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="n">
+      <c r="F1">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="n">
+      <c r="G1">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="n">
+      <c r="H1">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="n">
+      <c r="I1">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="n">
+      <c r="J1">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="n">
+      <c r="K1">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="n">
+      <c r="L1">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="n">
+      <c r="M1">
         <v>11</v>
       </c>
-      <c r="N1" s="0" t="n">
+      <c r="N1">
         <v>12</v>
       </c>
-      <c r="O1" s="0" t="n">
+      <c r="O1">
         <v>13</v>
       </c>
-      <c r="P1" s="0" t="n">
+      <c r="P1">
         <v>14</v>
       </c>
-      <c r="Q1" s="0" t="n">
+      <c r="Q1">
         <v>15</v>
       </c>
-      <c r="R1" s="0" t="n">
+      <c r="R1">
         <v>16</v>
       </c>
-      <c r="S1" s="0" t="n">
+      <c r="S1">
         <v>17</v>
       </c>
-      <c r="T1" s="0" t="n">
+      <c r="T1">
         <v>18</v>
       </c>
-      <c r="U1" s="0" t="n">
+      <c r="U1">
         <v>19</v>
       </c>
-      <c r="V1" s="0" t="n">
+      <c r="V1">
         <v>20</v>
       </c>
-      <c r="W1" s="0" t="n">
+      <c r="W1">
         <v>21</v>
       </c>
-      <c r="X1" s="0" t="n">
+      <c r="X1">
         <v>22</v>
       </c>
-      <c r="Y1" s="0" t="n">
+      <c r="Y1">
         <v>23</v>
       </c>
-      <c r="Z1" s="0" t="n">
+      <c r="Z1">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:26" ht="50" customHeight="1">
+      <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>145</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>144</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>143</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -429,8 +713,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:26" ht="50" customHeight="1">
+      <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -445,152 +729,152 @@
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>101</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>102</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>103</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3">
         <v>104</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3">
         <v>105</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3">
         <v>106</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3">
         <v>107</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3">
         <v>108</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3">
         <v>109</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3">
         <v>110</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3">
         <v>111</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3">
         <v>112</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3">
         <v>113</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3">
         <v>114</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3">
         <v>115</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3">
         <v>116</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3">
         <v>117</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3">
         <v>118</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3">
         <v>119</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3">
         <v>156</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:26" ht="50" customHeight="1">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>148</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4">
         <v>147</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>146</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>142</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="3">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="3">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="3">
         <v>12</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="J4" s="3">
         <v>13</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="3">
         <v>14</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="3">
         <v>15</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4">
         <v>153</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="3" t="n">
+      <c r="P4" s="3">
         <v>16</v>
       </c>
-      <c r="Q4" s="3" t="n">
+      <c r="Q4" s="3">
         <v>17</v>
       </c>
-      <c r="R4" s="3" t="n">
+      <c r="R4" s="3">
         <v>18</v>
       </c>
-      <c r="S4" s="3" t="n">
+      <c r="S4" s="3">
         <v>19</v>
       </c>
-      <c r="T4" s="3" t="n">
+      <c r="T4" s="3">
         <v>20</v>
       </c>
-      <c r="U4" s="3" t="n">
+      <c r="U4" s="3">
         <v>21</v>
       </c>
-      <c r="V4" s="3" t="n">
+      <c r="V4" s="3">
         <v>22</v>
       </c>
-      <c r="W4" s="3" t="n">
+      <c r="W4" s="3">
         <v>23</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4">
         <v>120</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4">
         <v>157</v>
       </c>
-      <c r="Z4" s="4" t="n">
+      <c r="Z4" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:26" ht="50" customHeight="1">
+      <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -605,215 +889,215 @@
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="5">
         <v>24</v>
       </c>
-      <c r="H5" s="5" t="n">
+      <c r="H5" s="5">
         <v>25</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="5">
         <v>26</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="5">
         <v>27</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="5">
         <v>28</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="5">
         <v>29</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5">
         <v>154</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="5" t="n">
+      <c r="P5" s="5">
         <v>30</v>
       </c>
-      <c r="Q5" s="5" t="n">
+      <c r="Q5" s="5">
         <v>31</v>
       </c>
-      <c r="R5" s="5" t="n">
+      <c r="R5" s="5">
         <v>32</v>
       </c>
-      <c r="S5" s="5" t="n">
+      <c r="S5" s="5">
         <v>33</v>
       </c>
-      <c r="T5" s="5" t="n">
+      <c r="T5" s="5">
         <v>34</v>
       </c>
-      <c r="U5" s="5" t="n">
+      <c r="U5" s="5">
         <v>35</v>
       </c>
-      <c r="V5" s="5" t="n">
+      <c r="V5" s="5">
         <v>36</v>
       </c>
-      <c r="W5" s="5" t="n">
+      <c r="W5" s="5">
         <v>37</v>
       </c>
-      <c r="X5" s="0" t="n">
+      <c r="X5">
         <v>121</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Y5">
         <v>158</v>
       </c>
-      <c r="Z5" s="4" t="n">
+      <c r="Z5" s="4">
         <v>501</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:26" ht="50" customHeight="1">
+      <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6">
         <v>150</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>149</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>141</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>140</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>139</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6">
         <v>138</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6">
         <v>137</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6">
         <v>136</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6">
         <v>135</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6">
         <v>134</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6">
         <v>133</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="O6">
         <v>132</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6">
         <v>131</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6">
         <v>130</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6">
         <v>129</v>
       </c>
-      <c r="S6" s="0" t="n">
+      <c r="S6">
         <v>128</v>
       </c>
-      <c r="T6" s="0" t="n">
+      <c r="T6">
         <v>127</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="U6">
         <v>126</v>
       </c>
-      <c r="V6" s="0" t="n">
+      <c r="V6">
         <v>125</v>
       </c>
-      <c r="W6" s="0" t="n">
+      <c r="W6">
         <v>124</v>
       </c>
-      <c r="X6" s="0" t="n">
+      <c r="X6">
         <v>122</v>
       </c>
-      <c r="Y6" s="0" t="n">
+      <c r="Y6">
         <v>159</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:26" ht="50" customHeight="1">
+      <c r="A7">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>152</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>151</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="3">
         <v>38</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="3">
         <v>39</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="3">
         <v>40</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="J7" s="3">
         <v>41</v>
       </c>
-      <c r="K7" s="3" t="n">
+      <c r="K7" s="3">
         <v>42</v>
       </c>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="3">
         <v>43</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="3">
         <v>44</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="3" t="n">
+      <c r="O7" s="3">
         <v>45</v>
       </c>
-      <c r="P7" s="3" t="n">
+      <c r="P7" s="3">
         <v>46</v>
       </c>
-      <c r="Q7" s="3" t="n">
+      <c r="Q7" s="3">
         <v>47</v>
       </c>
-      <c r="R7" s="3" t="n">
+      <c r="R7" s="3">
         <v>48</v>
       </c>
-      <c r="S7" s="3" t="n">
+      <c r="S7" s="3">
         <v>49</v>
       </c>
-      <c r="T7" s="3" t="n">
+      <c r="T7" s="3">
         <v>50</v>
       </c>
-      <c r="U7" s="3" t="n">
+      <c r="U7" s="3">
         <v>51</v>
       </c>
-      <c r="V7" s="3" t="n">
+      <c r="V7" s="3">
         <v>52</v>
       </c>
-      <c r="W7" s="3" t="n">
+      <c r="W7" s="3">
         <v>53</v>
       </c>
       <c r="X7" s="2" t="s">
@@ -826,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="50" customHeight="1">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -844,7 +1128,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="50" customHeight="1">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -862,7 +1146,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="50" customHeight="1">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -880,7 +1164,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="50" customHeight="1">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
@@ -898,7 +1182,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="50" customHeight="1">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -916,7 +1200,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="50" customHeight="1">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -935,12 +1219,8 @@
       <c r="Q13" s="9"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change node date & map
</commit_message>
<xml_diff>
--- a/cloudMap_v10.xlsx
+++ b/cloudMap_v10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/Documents/MAPF/MultiAgentPathFinder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F26C41-CAD7-4745-9FBD-B3958456F547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1A18F3-D34C-2F41-8AF2-95E6C70FA06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60160" yWindow="16340" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48000" yWindow="13080" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="2">
   <si>
     <t>axis</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="17"/>
@@ -553,7 +553,7 @@
     <col min="4" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,14 +626,8 @@
       <c r="X1">
         <v>22</v>
       </c>
-      <c r="Y1">
-        <v>23</v>
-      </c>
-      <c r="Z1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="50" customHeight="1">
+    </row>
+    <row r="2" spans="1:24" ht="50" customHeight="1">
       <c r="A2">
         <v>5</v>
       </c>
@@ -706,14 +700,8 @@
       <c r="X2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="50" customHeight="1">
+    </row>
+    <row r="3" spans="1:24" ht="50" customHeight="1">
       <c r="A3">
         <v>4</v>
       </c>
@@ -751,49 +739,43 @@
         <v>107</v>
       </c>
       <c r="M3">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N3">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="O3">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="P3">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Q3">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="R3">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="S3">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="T3">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="U3">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="V3">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="W3">
-        <v>118</v>
-      </c>
-      <c r="X3">
-        <v>119</v>
-      </c>
-      <c r="Y3">
         <v>156</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="50" customHeight="1">
+      <c r="X3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="50" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -830,50 +812,44 @@
       <c r="L4" s="3">
         <v>15</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4">
+      <c r="M4">
         <v>153</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>1</v>
+      <c r="N4" s="3">
+        <v>16</v>
+      </c>
+      <c r="O4" s="3">
+        <v>17</v>
       </c>
       <c r="P4" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="Q4" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R4" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="S4" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="T4" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U4" s="3">
-        <v>21</v>
-      </c>
-      <c r="V4" s="3">
-        <v>22</v>
-      </c>
-      <c r="W4" s="3">
         <v>23</v>
       </c>
-      <c r="X4">
+      <c r="V4">
         <v>120</v>
       </c>
-      <c r="Y4">
+      <c r="W4">
         <v>157</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="X4" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="50" customHeight="1">
+    <row r="5" spans="1:24" ht="50" customHeight="1">
       <c r="A5">
         <v>2</v>
       </c>
@@ -907,50 +883,44 @@
       <c r="L5" s="5">
         <v>29</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5">
+      <c r="M5">
         <v>154</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>1</v>
+      <c r="N5" s="5">
+        <v>30</v>
+      </c>
+      <c r="O5" s="5">
+        <v>31</v>
       </c>
       <c r="P5" s="5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q5" s="5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R5" s="5">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="S5" s="5">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T5" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="U5" s="5">
-        <v>35</v>
-      </c>
-      <c r="V5" s="5">
-        <v>36</v>
-      </c>
-      <c r="W5" s="5">
         <v>37</v>
       </c>
-      <c r="X5">
+      <c r="V5">
         <v>121</v>
       </c>
-      <c r="Y5">
+      <c r="W5">
         <v>158</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="X5" s="4">
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="50" customHeight="1">
+    <row r="6" spans="1:24" ht="50" customHeight="1">
       <c r="A6">
         <v>1</v>
       </c>
@@ -988,49 +958,43 @@
         <v>135</v>
       </c>
       <c r="M6">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N6">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O6">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P6">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q6">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R6">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="S6">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T6">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U6">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="V6">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="W6">
-        <v>124</v>
-      </c>
-      <c r="X6">
-        <v>122</v>
-      </c>
-      <c r="Y6">
         <v>159</v>
       </c>
-      <c r="Z6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="50" customHeight="1">
+      <c r="X6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="50" customHeight="1">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1067,50 +1031,44 @@
       <c r="L7" s="3">
         <v>43</v>
       </c>
-      <c r="M7" s="3">
-        <v>44</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>1</v>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>46</v>
       </c>
       <c r="O7" s="3">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P7" s="3">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q7" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R7" s="3">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S7" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T7" s="3">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U7" s="3">
-        <v>51</v>
-      </c>
-      <c r="V7" s="3">
-        <v>52</v>
-      </c>
-      <c r="W7" s="3">
         <v>53</v>
       </c>
+      <c r="V7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="X7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="50" customHeight="1">
+    </row>
+    <row r="8" spans="1:24" ht="50" customHeight="1">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1128,7 +1086,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
     </row>
-    <row r="9" spans="1:26" ht="50" customHeight="1">
+    <row r="9" spans="1:24" ht="50" customHeight="1">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
@@ -1146,7 +1104,7 @@
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
     </row>
-    <row r="10" spans="1:26" ht="50" customHeight="1">
+    <row r="10" spans="1:24" ht="50" customHeight="1">
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1164,7 +1122,7 @@
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
     </row>
-    <row r="11" spans="1:26" ht="50" customHeight="1">
+    <row r="11" spans="1:24" ht="50" customHeight="1">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
@@ -1182,7 +1140,7 @@
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
     </row>
-    <row r="12" spans="1:26" ht="50" customHeight="1">
+    <row r="12" spans="1:24" ht="50" customHeight="1">
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1200,7 +1158,7 @@
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
     </row>
-    <row r="13" spans="1:26" ht="50" customHeight="1">
+    <row r="13" spans="1:24" ht="50" customHeight="1">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>

</xml_diff>